<commit_message>
Atualização automática de FORO_REGIONAL_DO_ALTO_PETROPOLIS.xlsx
</commit_message>
<xml_diff>
--- a/FORO_REGIONAL_DO_ALTO_PETROPOLIS.xlsx
+++ b/FORO_REGIONAL_DO_ALTO_PETROPOLIS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8CB8DEC-DC97-4674-A839-77F4D50A5C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FC320B0-1032-4EE1-915F-2D9D207979E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1079,7 +1079,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{3861AA00-04FA-4550-80B3-8715EC86BCDA}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{82520C0B-DF61-4B69-98EA-CFE28B8AA6D5}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1109,10 +1109,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33B1EE6A-AE10-42B8-8118-D8958DBF8E55}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{760315E1-81AE-417D-BDD5-BC386D4FE45E}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1150,7 +1150,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69D0E6D9-014B-4DB5-BD92-15A50896439F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAA74684-7AFB-4563-A86F-373A3AAAE0FA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1213,7 +1213,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72EEE09C-95C1-4E67-997E-0A922C8BA4B0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F7C05FB-13E3-48C8-ABB8-E2A2F5242121}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1232,7 +1232,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D769EFC-405E-29FA-0CF3-6B87B6412F9B}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{205F0172-980D-2828-1C2A-1B38C274CFC9}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1281,7 +1281,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9961872D-9CAA-A2E0-B3F7-D23761B2357F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{028A3FC2-0FBF-6BFB-4C7B-D8DCECF72DE1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1300,7 +1300,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{170E33A3-E934-463A-37E2-ADF05588C279}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BD6214B-1DC1-5286-D513-5D73159BA2D8}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1331,7 +1331,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8D83C0E-BD82-B0D5-65DC-C6911977EAA1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C13731C7-7549-7958-994F-094F12E0AE6B}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1362,7 +1362,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C782DF6F-0941-9F24-6AF4-360F16848FE0}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC622B59-0E18-5EC3-039D-D66CA3D656EE}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1405,7 +1405,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12DFDF76-BF9F-4BEB-A877-F5145BD5FDF7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD4DC076-1950-447E-B088-695F3ECB4FA9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1443,7 +1443,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C41305D1-3DA5-4238-AD7B-CCAFD374E21B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0464D3B-37DB-4BCE-A44D-4F4A49BB4F0A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1486,7 +1486,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E232E9D8-8A1D-499F-8139-BC6EC0FD4584}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB431C6D-0A8D-4EC6-8404-7E7D110810D9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1799,7 +1799,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A42AC91-E7FA-47BF-8640-8157F1AE728D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1B87A59-6C83-4B90-98DC-8FEFA5D3CCB1}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>